<commit_message>
converted sigma to S/m
</commit_message>
<xml_diff>
--- a/sigma_standards_T_table.xlsx
+++ b/sigma_standards_T_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB319D\Desktop\Experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psarakis/HIPPOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B803C8-B489-41D0-B3E5-52401BEE308A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F3E715-46F5-CE47-B695-DA7BFFE7A427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{17922FDB-7F5E-4E6E-AE9E-242ECF0F2A20}"/>
+    <workbookView xWindow="11820" yWindow="5760" windowWidth="12860" windowHeight="14680" xr2:uid="{17922FDB-7F5E-4E6E-AE9E-242ECF0F2A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Standard (uS/cm) -&gt; Temp v</t>
   </si>
@@ -54,13 +62,22 @@
     <t>DI water in cup: 1.00 uS/cm</t>
   </si>
   <si>
-    <t>NIST sensor reading</t>
-  </si>
-  <si>
     <t>Percent difference</t>
   </si>
   <si>
     <t>Calibration 1</t>
+  </si>
+  <si>
+    <t>sigma_out (conductivity uS/cm)</t>
+  </si>
+  <si>
+    <t>NIST sensor reading (conductivity uS/cm)</t>
+  </si>
+  <si>
+    <t>sigma_out (conductivity S/m)</t>
+  </si>
+  <si>
+    <t>NIST sensor reading (conductivity S/m)</t>
   </si>
 </sst>
 </file>
@@ -110,7 +127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -155,11 +172,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -191,6 +234,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2517,7 +2566,7 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>419099</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2843,21 +2892,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6859A533-09BB-45EB-8D9C-28C9ED640C63}">
-  <dimension ref="A1:V36"/>
+  <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2878,12 +2927,12 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.2">
       <c r="V2">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2909,7 +2958,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>5</v>
       </c>
@@ -2939,7 +2988,7 @@
         <v>53.8</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>10</v>
       </c>
@@ -2969,7 +3018,7 @@
         <v>58.9</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>15</v>
       </c>
@@ -2999,7 +3048,7 @@
         <v>65.7</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>16</v>
       </c>
@@ -3029,7 +3078,7 @@
         <v>67.2</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>17</v>
       </c>
@@ -3059,7 +3108,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>18</v>
       </c>
@@ -3089,7 +3138,7 @@
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>19</v>
       </c>
@@ -3119,7 +3168,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>20</v>
       </c>
@@ -3149,7 +3198,7 @@
         <v>72.900000000000006</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>21</v>
       </c>
@@ -3179,7 +3228,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>22</v>
       </c>
@@ -3209,7 +3258,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>23</v>
       </c>
@@ -3239,7 +3288,7 @@
         <v>77.2</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>24</v>
       </c>
@@ -3269,7 +3318,7 @@
         <v>78.599999999999994</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>25</v>
       </c>
@@ -3299,7 +3348,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>26</v>
       </c>
@@ -3329,7 +3378,7 @@
         <v>81.599999999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>27</v>
       </c>
@@ -3359,7 +3408,7 @@
         <v>83.1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>28</v>
       </c>
@@ -3389,7 +3438,7 @@
         <v>84.7</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>29</v>
       </c>
@@ -3419,7 +3468,7 @@
         <v>86.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>30</v>
       </c>
@@ -3449,7 +3498,7 @@
         <v>87.7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>31</v>
       </c>
@@ -3479,12 +3528,12 @@
         <v>89.4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J23">
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -3513,7 +3562,7 @@
         <v>49002</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -3542,7 +3591,7 @@
         <v>1.9599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>6</v>
       </c>
@@ -3569,184 +3618,256 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="3">
+    <row r="28" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="6">
+        <f>C29*10^-4</f>
+        <v>2.1792110271198271E-3</v>
+      </c>
+      <c r="D28" s="6">
+        <f t="shared" ref="D28:I28" si="1">D29*10^-4</f>
+        <v>8.0625997196038524E-3</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="1"/>
+        <v>4.2277776222427225E-2</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="1"/>
+        <v>0.19260862635822734</v>
+      </c>
+      <c r="G28" s="6">
+        <f t="shared" si="1"/>
+        <v>0.25999281660369061</v>
+      </c>
+      <c r="H28" s="6">
+        <f t="shared" si="1"/>
+        <v>1.4017325171566899</v>
+      </c>
+      <c r="I28" s="6">
+        <f t="shared" si="1"/>
+        <v>7.6611034017929391</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="3">
         <f>IF(NOT(ISBLANK(C27)), C24*EXP(C25*C27), "")</f>
         <v>21.792110271198268</v>
       </c>
-      <c r="D28" s="3">
-        <f t="shared" ref="D28:I28" si="1">IF(NOT(ISBLANK(D27)), D24*EXP(D25*D27), "")</f>
+      <c r="D29" s="3">
+        <f t="shared" ref="D29:I29" si="2">IF(NOT(ISBLANK(D27)), D24*EXP(D25*D27), "")</f>
         <v>80.625997196038512</v>
       </c>
-      <c r="E28" s="3">
-        <f t="shared" si="1"/>
+      <c r="E29" s="3">
+        <f t="shared" si="2"/>
         <v>422.77776222427224</v>
       </c>
-      <c r="F28" s="3">
-        <f t="shared" si="1"/>
+      <c r="F29" s="3">
+        <f t="shared" si="2"/>
         <v>1926.0862635822732</v>
       </c>
-      <c r="G28" s="3">
-        <f t="shared" si="1"/>
+      <c r="G29" s="3">
+        <f t="shared" si="2"/>
         <v>2599.9281660369061</v>
       </c>
-      <c r="H28" s="3">
-        <f t="shared" si="1"/>
+      <c r="H29" s="3">
+        <f t="shared" si="2"/>
         <v>14017.325171566899</v>
       </c>
-      <c r="I28" s="3">
-        <f t="shared" si="1"/>
+      <c r="I29" s="3">
+        <f t="shared" si="2"/>
         <v>76611.034017929385</v>
       </c>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
     </row>
-    <row r="29" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+    <row r="30" spans="1:11" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="3">
+        <f>C31*10^-4</f>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" ref="D30:I30" si="3">D31*10^-4</f>
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="3"/>
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="3"/>
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="3"/>
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="H30" s="3">
+        <f t="shared" si="3"/>
+        <v>1.4590000000000001</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="3"/>
+        <v>7.8400000000000007</v>
+      </c>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="8">
+        <v>25</v>
+      </c>
+      <c r="D31" s="8">
+        <v>82</v>
+      </c>
+      <c r="E31" s="8">
+        <v>438</v>
+      </c>
+      <c r="F31" s="8">
+        <v>2010</v>
+      </c>
+      <c r="G31" s="8">
+        <v>2710</v>
+      </c>
+      <c r="H31" s="8">
+        <v>14590</v>
+      </c>
+      <c r="I31" s="8">
+        <v>78400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="8">
-        <v>25</v>
-      </c>
-      <c r="D29" s="8">
-        <v>82</v>
-      </c>
-      <c r="E29" s="8">
-        <v>438</v>
-      </c>
-      <c r="F29" s="8">
-        <v>2010</v>
-      </c>
-      <c r="G29" s="8">
-        <v>2710</v>
-      </c>
-      <c r="H29" s="8">
-        <v>14590</v>
-      </c>
-      <c r="I29" s="8">
-        <v>78400</v>
+      <c r="B32" s="12"/>
+      <c r="C32" s="9">
+        <f>(C31-C29)/C31*100</f>
+        <v>12.831558915206925</v>
+      </c>
+      <c r="D32" s="9">
+        <f t="shared" ref="D32:I32" si="4">(D31-D29)/D31*100</f>
+        <v>1.6756131755627908</v>
+      </c>
+      <c r="E32" s="9">
+        <f t="shared" si="4"/>
+        <v>3.4753967524492606</v>
+      </c>
+      <c r="F32" s="9">
+        <f t="shared" si="4"/>
+        <v>4.1748127571008355</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" si="4"/>
+        <v>4.0616912901510673</v>
+      </c>
+      <c r="H32" s="9">
+        <f t="shared" si="4"/>
+        <v>3.9251187692467484</v>
+      </c>
+      <c r="I32" s="9">
+        <f t="shared" si="4"/>
+        <v>2.2818443648859881</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="9">
-        <f>(C29-C28)/C29*100</f>
-        <v>12.831558915206925</v>
-      </c>
-      <c r="D30" s="9">
-        <f t="shared" ref="D30:I30" si="2">(D29-D28)/D29*100</f>
-        <v>1.6756131755627908</v>
-      </c>
-      <c r="E30" s="9">
-        <f t="shared" si="2"/>
-        <v>3.4753967524492606</v>
-      </c>
-      <c r="F30" s="9">
-        <f t="shared" si="2"/>
-        <v>4.1748127571008355</v>
-      </c>
-      <c r="G30" s="9">
-        <f t="shared" si="2"/>
-        <v>4.0616912901510673</v>
-      </c>
-      <c r="H30" s="9">
-        <f t="shared" si="2"/>
-        <v>3.9251187692467484</v>
-      </c>
-      <c r="I30" s="9">
-        <f t="shared" si="2"/>
-        <v>2.2818443648859881</v>
+      <c r="F36" s="2">
+        <v>2070</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2764</v>
+      </c>
+      <c r="H36" s="2">
+        <v>15000</v>
+      </c>
+      <c r="I36" s="2">
+        <v>80000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>8</v>
+    <row r="37" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6">
+        <v>23.3</v>
+      </c>
+      <c r="G37" s="6">
+        <v>23</v>
+      </c>
+      <c r="H37" s="6">
+        <v>22.7</v>
+      </c>
+      <c r="I37" s="6">
+        <v>22.7</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="2">
-        <v>2070</v>
-      </c>
-      <c r="G34" s="2">
-        <v>2764</v>
-      </c>
-      <c r="H34" s="2">
-        <v>15000</v>
-      </c>
-      <c r="I34" s="2">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6">
-        <v>23.3</v>
-      </c>
-      <c r="G35" s="6">
-        <v>23</v>
-      </c>
-      <c r="H35" s="6">
-        <v>22.7</v>
-      </c>
-      <c r="I35" s="6">
-        <v>22.7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+    <row r="38" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3">
-        <f t="shared" ref="F36:I36" si="3">IF(NOT(ISBLANK(F35)), F24*EXP(F25*F35), "")</f>
+      <c r="B38" s="10"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3">
+        <f t="shared" ref="F38:I38" si="5">IF(NOT(ISBLANK(F37)), F24*EXP(F25*F37), "")</f>
         <v>1969.2053807568627</v>
       </c>
-      <c r="G36" s="3">
-        <f t="shared" si="3"/>
+      <c r="G38" s="3">
+        <f t="shared" si="5"/>
         <v>2638.6140973673614</v>
       </c>
-      <c r="H36" s="3">
-        <f t="shared" si="3"/>
+      <c r="H38" s="3">
+        <f t="shared" si="5"/>
         <v>14047.916272625975</v>
       </c>
-      <c r="I36" s="3">
-        <f t="shared" si="3"/>
+      <c r="I38" s="3">
+        <f t="shared" si="5"/>
         <v>76461.023449634566</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A36:B36"/>
+  <mergeCells count="8">
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new sheet of sigma standards table for 2nd cal run
</commit_message>
<xml_diff>
--- a/sigma_standards_T_table.xlsx
+++ b/sigma_standards_T_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psarakis/HIPPOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB319D\Desktop\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F3E715-46F5-CE47-B695-DA7BFFE7A427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B803C8-B489-41D0-B3E5-52401BEE308A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="5760" windowWidth="12860" windowHeight="14680" xr2:uid="{17922FDB-7F5E-4E6E-AE9E-242ECF0F2A20}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{17922FDB-7F5E-4E6E-AE9E-242ECF0F2A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Standard (uS/cm) -&gt; Temp v</t>
   </si>
@@ -62,22 +54,13 @@
     <t>DI water in cup: 1.00 uS/cm</t>
   </si>
   <si>
+    <t>NIST sensor reading</t>
+  </si>
+  <si>
     <t>Percent difference</t>
   </si>
   <si>
     <t>Calibration 1</t>
-  </si>
-  <si>
-    <t>sigma_out (conductivity uS/cm)</t>
-  </si>
-  <si>
-    <t>NIST sensor reading (conductivity uS/cm)</t>
-  </si>
-  <si>
-    <t>sigma_out (conductivity S/m)</t>
-  </si>
-  <si>
-    <t>NIST sensor reading (conductivity S/m)</t>
   </si>
 </sst>
 </file>
@@ -127,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -172,37 +155,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -234,12 +191,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2566,7 +2517,7 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>419099</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2892,21 +2843,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6859A533-09BB-45EB-8D9C-28C9ED640C63}">
-  <dimension ref="A1:V38"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2927,12 +2878,12 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
       <c r="V2">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2958,7 +2909,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>5</v>
       </c>
@@ -2988,7 +2939,7 @@
         <v>53.8</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>10</v>
       </c>
@@ -3018,7 +2969,7 @@
         <v>58.9</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>15</v>
       </c>
@@ -3048,7 +2999,7 @@
         <v>65.7</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>16</v>
       </c>
@@ -3078,7 +3029,7 @@
         <v>67.2</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>17</v>
       </c>
@@ -3108,7 +3059,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>18</v>
       </c>
@@ -3138,7 +3089,7 @@
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>19</v>
       </c>
@@ -3168,7 +3119,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>20</v>
       </c>
@@ -3198,7 +3149,7 @@
         <v>72.900000000000006</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>21</v>
       </c>
@@ -3228,7 +3179,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>22</v>
       </c>
@@ -3258,7 +3209,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>23</v>
       </c>
@@ -3288,7 +3239,7 @@
         <v>77.2</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>24</v>
       </c>
@@ -3318,7 +3269,7 @@
         <v>78.599999999999994</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>25</v>
       </c>
@@ -3348,7 +3299,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>26</v>
       </c>
@@ -3378,7 +3329,7 @@
         <v>81.599999999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>27</v>
       </c>
@@ -3408,7 +3359,7 @@
         <v>83.1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>28</v>
       </c>
@@ -3438,7 +3389,7 @@
         <v>84.7</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>29</v>
       </c>
@@ -3468,7 +3419,7 @@
         <v>86.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>30</v>
       </c>
@@ -3498,7 +3449,7 @@
         <v>87.7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>31</v>
       </c>
@@ -3528,12 +3479,12 @@
         <v>89.4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J23">
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -3562,7 +3513,7 @@
         <v>49002</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -3591,7 +3542,7 @@
         <v>1.9599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>6</v>
       </c>
@@ -3618,256 +3569,184 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="6">
-        <f>C29*10^-4</f>
-        <v>2.1792110271198271E-3</v>
-      </c>
-      <c r="D28" s="6">
-        <f t="shared" ref="D28:I28" si="1">D29*10^-4</f>
-        <v>8.0625997196038524E-3</v>
-      </c>
-      <c r="E28" s="6">
-        <f t="shared" si="1"/>
-        <v>4.2277776222427225E-2</v>
-      </c>
-      <c r="F28" s="6">
-        <f t="shared" si="1"/>
-        <v>0.19260862635822734</v>
-      </c>
-      <c r="G28" s="6">
-        <f t="shared" si="1"/>
-        <v>0.25999281660369061</v>
-      </c>
-      <c r="H28" s="6">
-        <f t="shared" si="1"/>
-        <v>1.4017325171566899</v>
-      </c>
-      <c r="I28" s="6">
-        <f t="shared" si="1"/>
-        <v>7.6611034017929391</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="3">
+    <row r="28" spans="1:11" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="3">
         <f>IF(NOT(ISBLANK(C27)), C24*EXP(C25*C27), "")</f>
         <v>21.792110271198268</v>
       </c>
-      <c r="D29" s="3">
-        <f t="shared" ref="D29:I29" si="2">IF(NOT(ISBLANK(D27)), D24*EXP(D25*D27), "")</f>
+      <c r="D28" s="3">
+        <f t="shared" ref="D28:I28" si="1">IF(NOT(ISBLANK(D27)), D24*EXP(D25*D27), "")</f>
         <v>80.625997196038512</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E28" s="3">
+        <f t="shared" si="1"/>
+        <v>422.77776222427224</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="1"/>
+        <v>1926.0862635822732</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" si="1"/>
+        <v>2599.9281660369061</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="1"/>
+        <v>14017.325171566899</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="1"/>
+        <v>76611.034017929385</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="8">
+        <v>25</v>
+      </c>
+      <c r="D29" s="8">
+        <v>82</v>
+      </c>
+      <c r="E29" s="8">
+        <v>438</v>
+      </c>
+      <c r="F29" s="8">
+        <v>2010</v>
+      </c>
+      <c r="G29" s="8">
+        <v>2710</v>
+      </c>
+      <c r="H29" s="8">
+        <v>14590</v>
+      </c>
+      <c r="I29" s="8">
+        <v>78400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="9">
+        <f>(C29-C28)/C29*100</f>
+        <v>12.831558915206925</v>
+      </c>
+      <c r="D30" s="9">
+        <f t="shared" ref="D30:I30" si="2">(D29-D28)/D29*100</f>
+        <v>1.6756131755627908</v>
+      </c>
+      <c r="E30" s="9">
         <f t="shared" si="2"/>
-        <v>422.77776222427224</v>
-      </c>
-      <c r="F29" s="3">
+        <v>3.4753967524492606</v>
+      </c>
+      <c r="F30" s="9">
         <f t="shared" si="2"/>
-        <v>1926.0862635822732</v>
-      </c>
-      <c r="G29" s="3">
+        <v>4.1748127571008355</v>
+      </c>
+      <c r="G30" s="9">
         <f t="shared" si="2"/>
-        <v>2599.9281660369061</v>
-      </c>
-      <c r="H29" s="3">
+        <v>4.0616912901510673</v>
+      </c>
+      <c r="H30" s="9">
         <f t="shared" si="2"/>
-        <v>14017.325171566899</v>
-      </c>
-      <c r="I29" s="3">
+        <v>3.9251187692467484</v>
+      </c>
+      <c r="I30" s="9">
         <f t="shared" si="2"/>
-        <v>76611.034017929385</v>
-      </c>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+        <v>2.2818443648859881</v>
+      </c>
     </row>
-    <row r="30" spans="1:11" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="3">
-        <f>C31*10^-4</f>
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" ref="D30:I30" si="3">D31*10^-4</f>
-        <v>8.2000000000000007E-3</v>
-      </c>
-      <c r="E30" s="3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="2">
+        <v>2070</v>
+      </c>
+      <c r="G34" s="2">
+        <v>2764</v>
+      </c>
+      <c r="H34" s="2">
+        <v>15000</v>
+      </c>
+      <c r="I34" s="2">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6">
+        <v>23.3</v>
+      </c>
+      <c r="G35" s="6">
+        <v>23</v>
+      </c>
+      <c r="H35" s="6">
+        <v>22.7</v>
+      </c>
+      <c r="I35" s="6">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3">
+        <f t="shared" ref="F36:I36" si="3">IF(NOT(ISBLANK(F35)), F24*EXP(F25*F35), "")</f>
+        <v>1969.2053807568627</v>
+      </c>
+      <c r="G36" s="3">
         <f t="shared" si="3"/>
-        <v>4.3799999999999999E-2</v>
-      </c>
-      <c r="F30" s="3">
+        <v>2638.6140973673614</v>
+      </c>
+      <c r="H36" s="3">
         <f t="shared" si="3"/>
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="G30" s="3">
+        <v>14047.916272625975</v>
+      </c>
+      <c r="I36" s="3">
         <f t="shared" si="3"/>
-        <v>0.27100000000000002</v>
-      </c>
-      <c r="H30" s="3">
-        <f t="shared" si="3"/>
-        <v>1.4590000000000001</v>
-      </c>
-      <c r="I30" s="3">
-        <f t="shared" si="3"/>
-        <v>7.8400000000000007</v>
-      </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="8">
-        <v>25</v>
-      </c>
-      <c r="D31" s="8">
-        <v>82</v>
-      </c>
-      <c r="E31" s="8">
-        <v>438</v>
-      </c>
-      <c r="F31" s="8">
-        <v>2010</v>
-      </c>
-      <c r="G31" s="8">
-        <v>2710</v>
-      </c>
-      <c r="H31" s="8">
-        <v>14590</v>
-      </c>
-      <c r="I31" s="8">
-        <v>78400</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="9">
-        <f>(C31-C29)/C31*100</f>
-        <v>12.831558915206925</v>
-      </c>
-      <c r="D32" s="9">
-        <f t="shared" ref="D32:I32" si="4">(D31-D29)/D31*100</f>
-        <v>1.6756131755627908</v>
-      </c>
-      <c r="E32" s="9">
-        <f t="shared" si="4"/>
-        <v>3.4753967524492606</v>
-      </c>
-      <c r="F32" s="9">
-        <f t="shared" si="4"/>
-        <v>4.1748127571008355</v>
-      </c>
-      <c r="G32" s="9">
-        <f t="shared" si="4"/>
-        <v>4.0616912901510673</v>
-      </c>
-      <c r="H32" s="9">
-        <f t="shared" si="4"/>
-        <v>3.9251187692467484</v>
-      </c>
-      <c r="I32" s="9">
-        <f t="shared" si="4"/>
-        <v>2.2818443648859881</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="2">
-        <v>2070</v>
-      </c>
-      <c r="G36" s="2">
-        <v>2764</v>
-      </c>
-      <c r="H36" s="2">
-        <v>15000</v>
-      </c>
-      <c r="I36" s="2">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6">
-        <v>23.3</v>
-      </c>
-      <c r="G37" s="6">
-        <v>23</v>
-      </c>
-      <c r="H37" s="6">
-        <v>22.7</v>
-      </c>
-      <c r="I37" s="6">
-        <v>22.7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3">
-        <f t="shared" ref="F38:I38" si="5">IF(NOT(ISBLANK(F37)), F24*EXP(F25*F37), "")</f>
-        <v>1969.2053807568627</v>
-      </c>
-      <c r="G38" s="3">
-        <f t="shared" si="5"/>
-        <v>2638.6140973673614</v>
-      </c>
-      <c r="H38" s="3">
-        <f t="shared" si="5"/>
-        <v>14047.916272625975</v>
-      </c>
-      <c r="I38" s="3">
-        <f t="shared" si="5"/>
         <v>76461.023449634566</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A38:B38"/>
+  <mergeCells count="6">
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A27:B27"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed extra copy of standards spreadsheet and added sheet from 2nd cal run
</commit_message>
<xml_diff>
--- a/sigma_standards_T_table.xlsx
+++ b/sigma_standards_T_table.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB319D\Desktop\Experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB319D\gitHIPPOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B803C8-B489-41D0-B3E5-52401BEE308A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1247FDE-AE5E-4861-B096-821AE204E65F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{17922FDB-7F5E-4E6E-AE9E-242ECF0F2A20}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{17922FDB-7F5E-4E6E-AE9E-242ECF0F2A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="06-24-22" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>Standard (uS/cm) -&gt; Temp v</t>
   </si>
@@ -61,6 +62,9 @@
   </si>
   <si>
     <t>Calibration 1</t>
+  </si>
+  <si>
+    <t>DI water in cup: 1.72uS/cm</t>
   </si>
 </sst>
 </file>
@@ -225,35 +229,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Conductivity</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of standards vs. T (C)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1758,6 +1733,1716 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-577D-47F0-B15B-82C7E37F81C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="767553663"/>
+        <c:axId val="675064063"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="767553663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="675064063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="675064063"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="767553663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.9913510811148604E-2"/>
+          <c:y val="7.0800252047889117E-2"/>
+          <c:w val="0.87773728283964503"/>
+          <c:h val="0.84804469384616143"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$C$4:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>15.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.51</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23.43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24.56</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25.61</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D960-47FD-A0A6-A5570EBFA17A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$D$4:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D960-47FD-A0A6-A5570EBFA17A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$E$4:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>411</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>447</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>467</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>477</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>487</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>505</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D960-47FD-A0A6-A5570EBFA17A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$F$4:$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1230</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1418</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1613</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1652</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1689</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1723</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1777</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1830</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1870</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1920</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1970</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2070</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2110</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2290</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2340</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-D960-47FD-A0A6-A5570EBFA17A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$G$4:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1752</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2244</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2296</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2346</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2448</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2502</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2554</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2606</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2658</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2712</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2764</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2816</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2872</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2922</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2952</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3030</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3082</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-D960-47FD-A0A6-A5570EBFA17A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$H$4:$H$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>9430</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12050</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12280</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12590</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13190</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13510</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13810</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14090</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14350</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14690</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15280</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15510</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15820</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16130</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16450</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16770</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-D960-47FD-A0A6-A5570EBFA17A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'06-24-22'!$I$4:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>53800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58900</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65700</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68700</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74300</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>75800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>77200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>78600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>81600</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>83100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>84700</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>86200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>87700</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-D960-47FD-A0A6-A5570EBFA17A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1989,7 +3674,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2546,6 +4787,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>447674</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF575997-2DA6-4374-A629-39452B7C9A22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2845,8 +5129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6859A533-09BB-45EB-8D9C-28C9ED640C63}">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3638,32 +5922,32 @@
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="9">
-        <f>(C29-C28)/C29*100</f>
-        <v>12.831558915206925</v>
+        <f>(100*C29/C28)-100</f>
+        <v>14.720418026892361</v>
       </c>
       <c r="D30" s="9">
-        <f t="shared" ref="D30:I30" si="2">(D29-D28)/D29*100</f>
-        <v>1.6756131755627908</v>
+        <f t="shared" ref="D30:I30" si="2">(100*D29/D28)-100</f>
+        <v>1.7041684465876017</v>
       </c>
       <c r="E30" s="9">
         <f t="shared" si="2"/>
-        <v>3.4753967524492606</v>
+        <v>3.6005294355223896</v>
       </c>
       <c r="F30" s="9">
         <f t="shared" si="2"/>
-        <v>4.1748127571008355</v>
+        <v>4.3566966861420866</v>
       </c>
       <c r="G30" s="9">
         <f t="shared" si="2"/>
-        <v>4.0616912901510673</v>
+        <v>4.233649044653319</v>
       </c>
       <c r="H30" s="9">
         <f t="shared" si="2"/>
-        <v>3.9251187692467484</v>
+        <v>4.0854786589008398</v>
       </c>
       <c r="I30" s="9">
         <f t="shared" si="2"/>
-        <v>2.2818443648859881</v>
+        <v>2.3351283597764052</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3752,4 +6036,920 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1B8C85-3DA4-434F-83AF-5F1A19563F16}">
+  <dimension ref="A1:V36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2">
+        <v>84</v>
+      </c>
+      <c r="E3" s="2">
+        <v>447</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2070</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2764</v>
+      </c>
+      <c r="H3" s="2">
+        <v>15000</v>
+      </c>
+      <c r="I3" s="2">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>15.32</v>
+      </c>
+      <c r="D4">
+        <v>65</v>
+      </c>
+      <c r="E4">
+        <v>278</v>
+      </c>
+      <c r="F4">
+        <v>1230</v>
+      </c>
+      <c r="G4">
+        <v>1752</v>
+      </c>
+      <c r="H4">
+        <v>9430</v>
+      </c>
+      <c r="I4">
+        <f>J4*$J$23</f>
+        <v>53800</v>
+      </c>
+      <c r="J4">
+        <v>53.8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>17.11</v>
+      </c>
+      <c r="D5">
+        <v>67</v>
+      </c>
+      <c r="E5">
+        <v>318</v>
+      </c>
+      <c r="F5">
+        <v>1418</v>
+      </c>
+      <c r="G5">
+        <v>1998</v>
+      </c>
+      <c r="H5">
+        <v>10720</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I22" si="0">J5*$J$23</f>
+        <v>58900</v>
+      </c>
+      <c r="J5">
+        <v>58.9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>18.32</v>
+      </c>
+      <c r="D6">
+        <v>68</v>
+      </c>
+      <c r="E6">
+        <v>361</v>
+      </c>
+      <c r="F6">
+        <v>1613</v>
+      </c>
+      <c r="G6">
+        <v>2244</v>
+      </c>
+      <c r="H6">
+        <v>12050</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>65700</v>
+      </c>
+      <c r="J6">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>18.649999999999999</v>
+      </c>
+      <c r="D7">
+        <v>70</v>
+      </c>
+      <c r="E7">
+        <v>368</v>
+      </c>
+      <c r="F7">
+        <v>1652</v>
+      </c>
+      <c r="G7">
+        <v>2296</v>
+      </c>
+      <c r="H7">
+        <v>12280</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>67200</v>
+      </c>
+      <c r="J7">
+        <v>67.2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>18.97</v>
+      </c>
+      <c r="D8">
+        <v>71</v>
+      </c>
+      <c r="E8">
+        <v>376</v>
+      </c>
+      <c r="F8">
+        <v>1689</v>
+      </c>
+      <c r="G8">
+        <v>2346</v>
+      </c>
+      <c r="H8">
+        <v>12590</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>68700</v>
+      </c>
+      <c r="J8">
+        <v>68.7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>19.41</v>
+      </c>
+      <c r="D9">
+        <v>73</v>
+      </c>
+      <c r="E9">
+        <v>385</v>
+      </c>
+      <c r="F9">
+        <v>1723</v>
+      </c>
+      <c r="G9">
+        <v>2400</v>
+      </c>
+      <c r="H9">
+        <v>12900</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>70100</v>
+      </c>
+      <c r="J9">
+        <v>70.099999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="D10">
+        <v>74</v>
+      </c>
+      <c r="E10">
+        <v>394</v>
+      </c>
+      <c r="F10">
+        <v>1777</v>
+      </c>
+      <c r="G10">
+        <v>2448</v>
+      </c>
+      <c r="H10">
+        <v>13190</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>71500</v>
+      </c>
+      <c r="J10">
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>20.3</v>
+      </c>
+      <c r="D11">
+        <v>76</v>
+      </c>
+      <c r="E11">
+        <v>402</v>
+      </c>
+      <c r="F11">
+        <v>1830</v>
+      </c>
+      <c r="G11">
+        <v>2502</v>
+      </c>
+      <c r="H11">
+        <v>13510</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>72900</v>
+      </c>
+      <c r="J11">
+        <v>72.900000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>20.92</v>
+      </c>
+      <c r="D12">
+        <v>78</v>
+      </c>
+      <c r="E12">
+        <v>411</v>
+      </c>
+      <c r="F12">
+        <v>1870</v>
+      </c>
+      <c r="G12">
+        <v>2554</v>
+      </c>
+      <c r="H12">
+        <v>13810</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>74300</v>
+      </c>
+      <c r="J12">
+        <v>74.3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>21.51</v>
+      </c>
+      <c r="D13">
+        <v>79</v>
+      </c>
+      <c r="E13">
+        <v>419</v>
+      </c>
+      <c r="F13">
+        <v>1920</v>
+      </c>
+      <c r="G13">
+        <v>2606</v>
+      </c>
+      <c r="H13">
+        <v>14090</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>75800</v>
+      </c>
+      <c r="J13">
+        <v>75.8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>22.1</v>
+      </c>
+      <c r="D14">
+        <v>81</v>
+      </c>
+      <c r="E14">
+        <v>430</v>
+      </c>
+      <c r="F14">
+        <v>1970</v>
+      </c>
+      <c r="G14">
+        <v>2658</v>
+      </c>
+      <c r="H14">
+        <v>14350</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>77200</v>
+      </c>
+      <c r="J14">
+        <v>77.2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>22.55</v>
+      </c>
+      <c r="D15">
+        <v>82</v>
+      </c>
+      <c r="E15">
+        <v>438</v>
+      </c>
+      <c r="F15">
+        <v>2020</v>
+      </c>
+      <c r="G15">
+        <v>2712</v>
+      </c>
+      <c r="H15">
+        <v>14690</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>78600</v>
+      </c>
+      <c r="J15">
+        <v>78.599999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>23</v>
+      </c>
+      <c r="D16">
+        <v>84</v>
+      </c>
+      <c r="E16">
+        <v>447</v>
+      </c>
+      <c r="F16">
+        <v>2070</v>
+      </c>
+      <c r="G16">
+        <v>2764</v>
+      </c>
+      <c r="H16">
+        <v>15000</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
+      <c r="J16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>23.43</v>
+      </c>
+      <c r="D17">
+        <v>86</v>
+      </c>
+      <c r="E17">
+        <v>457</v>
+      </c>
+      <c r="F17">
+        <v>2110</v>
+      </c>
+      <c r="G17">
+        <v>2816</v>
+      </c>
+      <c r="H17">
+        <v>15280</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>81600</v>
+      </c>
+      <c r="J17">
+        <v>81.599999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>23.9</v>
+      </c>
+      <c r="D18">
+        <v>87</v>
+      </c>
+      <c r="E18">
+        <v>467</v>
+      </c>
+      <c r="F18">
+        <v>2150</v>
+      </c>
+      <c r="G18">
+        <v>2872</v>
+      </c>
+      <c r="H18">
+        <v>15510</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>83100</v>
+      </c>
+      <c r="J18">
+        <v>83.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>24.56</v>
+      </c>
+      <c r="D19">
+        <v>89</v>
+      </c>
+      <c r="E19">
+        <v>477</v>
+      </c>
+      <c r="F19">
+        <v>2200</v>
+      </c>
+      <c r="G19">
+        <v>2922</v>
+      </c>
+      <c r="H19">
+        <v>15820</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>84700</v>
+      </c>
+      <c r="J19">
+        <v>84.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>29</v>
+      </c>
+      <c r="C20">
+        <v>25.2</v>
+      </c>
+      <c r="D20">
+        <v>90</v>
+      </c>
+      <c r="E20">
+        <v>487</v>
+      </c>
+      <c r="F20">
+        <v>2250</v>
+      </c>
+      <c r="G20">
+        <v>2952</v>
+      </c>
+      <c r="H20">
+        <v>16130</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>86200</v>
+      </c>
+      <c r="J20">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>30</v>
+      </c>
+      <c r="C21">
+        <v>25.61</v>
+      </c>
+      <c r="D21">
+        <v>92</v>
+      </c>
+      <c r="E21">
+        <v>496</v>
+      </c>
+      <c r="F21">
+        <v>2290</v>
+      </c>
+      <c r="G21">
+        <v>3030</v>
+      </c>
+      <c r="H21">
+        <v>16450</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>87700</v>
+      </c>
+      <c r="J21">
+        <v>87.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>26.4</v>
+      </c>
+      <c r="D22">
+        <v>94</v>
+      </c>
+      <c r="E22">
+        <v>505</v>
+      </c>
+      <c r="F22">
+        <v>2340</v>
+      </c>
+      <c r="G22">
+        <v>3082</v>
+      </c>
+      <c r="H22">
+        <v>16770</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>89400</v>
+      </c>
+      <c r="J22">
+        <v>89.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>13.465999999999999</v>
+      </c>
+      <c r="D24">
+        <v>55.853999999999999</v>
+      </c>
+      <c r="E24">
+        <v>254.83</v>
+      </c>
+      <c r="F24">
+        <v>1110.0999999999999</v>
+      </c>
+      <c r="G24">
+        <v>1624.1</v>
+      </c>
+      <c r="H24">
+        <v>8564.4</v>
+      </c>
+      <c r="I24">
+        <v>49002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="D25">
+        <v>1.61E-2</v>
+      </c>
+      <c r="E25">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="F25">
+        <v>2.46E-2</v>
+      </c>
+      <c r="G25">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="H25">
+        <v>2.18E-2</v>
+      </c>
+      <c r="I25">
+        <v>1.9599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="6">
+        <v>22.8</v>
+      </c>
+      <c r="D27" s="6">
+        <v>22.3</v>
+      </c>
+      <c r="E27" s="6">
+        <v>21.7</v>
+      </c>
+      <c r="F27" s="6">
+        <v>21.5</v>
+      </c>
+      <c r="G27" s="6">
+        <v>21.7</v>
+      </c>
+      <c r="H27" s="6">
+        <v>21.8</v>
+      </c>
+      <c r="I27" s="6">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="8">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="D28" s="8">
+        <v>87.8</v>
+      </c>
+      <c r="E28" s="8">
+        <v>426</v>
+      </c>
+      <c r="F28" s="8">
+        <v>1959</v>
+      </c>
+      <c r="G28" s="8">
+        <v>2630</v>
+      </c>
+      <c r="H28" s="8">
+        <v>13920</v>
+      </c>
+      <c r="I28" s="8">
+        <v>75200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="3">
+        <f>IF(NOT(ISBLANK(C27)), C24*EXP(C25*C27), "")</f>
+        <v>21.885142679289942</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" ref="D29:I29" si="1">IF(NOT(ISBLANK(D27)), D24*EXP(D25*D27), "")</f>
+        <v>79.979563305892157</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="1"/>
+        <v>415.23584340432336</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="1"/>
+        <v>1883.9113131685938</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="1"/>
+        <v>2567.220551506402</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" si="1"/>
+        <v>13774.982392033568</v>
+      </c>
+      <c r="I29" s="3">
+        <f t="shared" si="1"/>
+        <v>75271.465111520898</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="9">
+        <f t="shared" ref="C30:I30" si="2">(100*C28/C29)-100</f>
+        <v>63.581295880139635</v>
+      </c>
+      <c r="D30" s="9">
+        <f t="shared" si="2"/>
+        <v>9.7780437537494151</v>
+      </c>
+      <c r="E30" s="9">
+        <f t="shared" si="2"/>
+        <v>2.5922994767085612</v>
+      </c>
+      <c r="F30" s="9">
+        <f t="shared" si="2"/>
+        <v>3.9857867144028631</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" si="2"/>
+        <v>2.4454248177765692</v>
+      </c>
+      <c r="H30" s="9">
+        <f t="shared" si="2"/>
+        <v>1.0527607501719984</v>
+      </c>
+      <c r="I30" s="9">
+        <f t="shared" si="2"/>
+        <v>-9.4943165268560392E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="2">
+        <v>2070</v>
+      </c>
+      <c r="G34" s="2">
+        <v>2764</v>
+      </c>
+      <c r="H34" s="2">
+        <v>15000</v>
+      </c>
+      <c r="I34" s="2">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6">
+        <v>23.3</v>
+      </c>
+      <c r="G35" s="6">
+        <v>23</v>
+      </c>
+      <c r="H35" s="6">
+        <v>22.7</v>
+      </c>
+      <c r="I35" s="6">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3">
+        <f>IF(NOT(ISBLANK(F35)), F24*EXP(F25*F35), "")</f>
+        <v>1969.2053807568627</v>
+      </c>
+      <c r="G36" s="3">
+        <f>IF(NOT(ISBLANK(G35)), G24*EXP(G25*G35), "")</f>
+        <v>2638.6140973673614</v>
+      </c>
+      <c r="H36" s="3">
+        <f>IF(NOT(ISBLANK(H35)), H24*EXP(H25*H35), "")</f>
+        <v>14047.916272625975</v>
+      </c>
+      <c r="I36" s="3">
+        <f>IF(NOT(ISBLANK(I35)), I24*EXP(I25*I35), "")</f>
+        <v>76461.023449634566</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A35:B35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added 2764 uS/cm durability test P ramp data
</commit_message>
<xml_diff>
--- a/sigma_standards_T_table.xlsx
+++ b/sigma_standards_T_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB319D\gitHIPPOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1247FDE-AE5E-4861-B096-821AE204E65F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47761D1-E593-4315-8A98-8AD423B0FD03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{17922FDB-7F5E-4E6E-AE9E-242ECF0F2A20}"/>
   </bookViews>
@@ -6042,8 +6042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1B8C85-3DA4-434F-83AF-5F1A19563F16}">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6757,7 +6757,8 @@
         <v>21.5</v>
       </c>
       <c r="G27" s="6">
-        <v>21.7</v>
+        <f>296.365-273.15</f>
+        <v>23.215000000000032</v>
       </c>
       <c r="H27" s="6">
         <v>21.8</v>
@@ -6816,7 +6817,7 @@
       </c>
       <c r="G29" s="3">
         <f t="shared" si="1"/>
-        <v>2567.220551506402</v>
+        <v>2650.6113624414397</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="1"/>
@@ -6852,7 +6853,7 @@
       </c>
       <c r="G30" s="9">
         <f t="shared" si="2"/>
-        <v>2.4454248177765692</v>
+        <v>-0.77760786562292594</v>
       </c>
       <c r="H30" s="9">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Updated Excel spreadsheet fits to be in terms of K
</commit_message>
<xml_diff>
--- a/sigma_standards_T_table.xlsx
+++ b/sigma_standards_T_table.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB319D\gitHIPPOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjstyczi/HIPPOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47761D1-E593-4315-8A98-8AD423B0FD03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBB38E2-CFAD-1247-B1A1-01F98D813769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{17922FDB-7F5E-4E6E-AE9E-242ECF0F2A20}"/>
+    <workbookView xWindow="17060" yWindow="500" windowWidth="18560" windowHeight="19820" activeTab="1" xr2:uid="{17922FDB-7F5E-4E6E-AE9E-242ECF0F2A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="06-24-22" sheetId="2" r:id="rId2"/>
+    <sheet name="P conversion" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Standard (uS/cm) -&gt; Temp v</t>
   </si>
@@ -66,6 +75,24 @@
   <si>
     <t>DI water in cup: 1.72uS/cm</t>
   </si>
+  <si>
+    <t>Pressure conversion table</t>
+  </si>
+  <si>
+    <t>Low PSI</t>
+  </si>
+  <si>
+    <t>High MPa</t>
+  </si>
+  <si>
+    <t>High PSI</t>
+  </si>
+  <si>
+    <t>High bar</t>
+  </si>
+  <si>
+    <t>Temp in K</t>
+  </si>
 </sst>
 </file>
 
@@ -74,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,16 +132,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -159,11 +237,248 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -188,6 +503,33 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -195,6 +537,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1987,6 +2335,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-24-22'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -2055,66 +2414,66 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:f>'06-24-22'!$A$4:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>278.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>283.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>288.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>289.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>290.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>291.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>292.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>293.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>294.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>295.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>296.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>297.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>298.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>299.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27</c:v>
+                  <c:v>300.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28</c:v>
+                  <c:v>301.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29</c:v>
+                  <c:v>302.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30</c:v>
+                  <c:v>303.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31</c:v>
+                  <c:v>304.14999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2195,6 +2554,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-24-22'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>84</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -2263,66 +2633,66 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:f>'06-24-22'!$A$4:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>278.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>283.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>288.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>289.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>290.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>291.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>292.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>293.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>294.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>295.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>296.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>297.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>298.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>299.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27</c:v>
+                  <c:v>300.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28</c:v>
+                  <c:v>301.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29</c:v>
+                  <c:v>302.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30</c:v>
+                  <c:v>303.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31</c:v>
+                  <c:v>304.14999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2403,6 +2773,17 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-24-22'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>447</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -2471,66 +2852,66 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:f>'06-24-22'!$A$4:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>278.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>283.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>288.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>289.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>290.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>291.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>292.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>293.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>294.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>295.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>296.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>297.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>298.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>299.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27</c:v>
+                  <c:v>300.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28</c:v>
+                  <c:v>301.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29</c:v>
+                  <c:v>302.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30</c:v>
+                  <c:v>303.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31</c:v>
+                  <c:v>304.14999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2611,6 +2992,17 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-24-22'!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2070</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -2679,66 +3071,66 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:f>'06-24-22'!$A$4:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>278.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>283.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>288.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>289.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>290.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>291.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>292.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>293.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>294.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>295.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>296.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>297.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>298.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>299.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27</c:v>
+                  <c:v>300.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28</c:v>
+                  <c:v>301.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29</c:v>
+                  <c:v>302.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30</c:v>
+                  <c:v>303.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31</c:v>
+                  <c:v>304.14999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2819,6 +3211,17 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-24-22'!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2764</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -2887,66 +3290,66 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:f>'06-24-22'!$A$4:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>278.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>283.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>288.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>289.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>290.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>291.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>292.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>293.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>294.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>295.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>296.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>297.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>298.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>299.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27</c:v>
+                  <c:v>300.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28</c:v>
+                  <c:v>301.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29</c:v>
+                  <c:v>302.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30</c:v>
+                  <c:v>303.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31</c:v>
+                  <c:v>304.14999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3027,6 +3430,17 @@
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-24-22'!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>15000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -3095,66 +3509,66 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:f>'06-24-22'!$A$4:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>278.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>283.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>288.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>289.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>290.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>291.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>292.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>293.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>294.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>295.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>296.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>297.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>298.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>299.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27</c:v>
+                  <c:v>300.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28</c:v>
+                  <c:v>301.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29</c:v>
+                  <c:v>302.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30</c:v>
+                  <c:v>303.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31</c:v>
+                  <c:v>304.14999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3235,6 +3649,17 @@
         <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'06-24-22'!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -3309,66 +3734,66 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'06-24-22'!$B$4:$B$22</c:f>
+              <c:f>'06-24-22'!$A$4:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>278.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>283.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>288.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>289.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>290.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>291.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>292.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>293.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>294.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>295.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>296.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24</c:v>
+                  <c:v>297.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>298.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>299.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27</c:v>
+                  <c:v>300.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28</c:v>
+                  <c:v>301.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29</c:v>
+                  <c:v>302.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30</c:v>
+                  <c:v>303.14999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31</c:v>
+                  <c:v>304.14999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5133,15 +5558,15 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5162,12 +5587,12 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.2">
       <c r="V2">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -5193,7 +5618,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>5</v>
       </c>
@@ -5223,7 +5648,7 @@
         <v>53.8</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>10</v>
       </c>
@@ -5253,7 +5678,7 @@
         <v>58.9</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>15</v>
       </c>
@@ -5283,7 +5708,7 @@
         <v>65.7</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>16</v>
       </c>
@@ -5313,7 +5738,7 @@
         <v>67.2</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>17</v>
       </c>
@@ -5343,7 +5768,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>18</v>
       </c>
@@ -5373,7 +5798,7 @@
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>19</v>
       </c>
@@ -5403,7 +5828,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>20</v>
       </c>
@@ -5433,7 +5858,7 @@
         <v>72.900000000000006</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>21</v>
       </c>
@@ -5463,7 +5888,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>22</v>
       </c>
@@ -5493,7 +5918,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>23</v>
       </c>
@@ -5523,7 +5948,7 @@
         <v>77.2</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>24</v>
       </c>
@@ -5553,7 +5978,7 @@
         <v>78.599999999999994</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>25</v>
       </c>
@@ -5583,7 +6008,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>26</v>
       </c>
@@ -5613,7 +6038,7 @@
         <v>81.599999999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>27</v>
       </c>
@@ -5643,7 +6068,7 @@
         <v>83.1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>28</v>
       </c>
@@ -5673,7 +6098,7 @@
         <v>84.7</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>29</v>
       </c>
@@ -5703,7 +6128,7 @@
         <v>86.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>30</v>
       </c>
@@ -5733,7 +6158,7 @@
         <v>87.7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>31</v>
       </c>
@@ -5763,12 +6188,12 @@
         <v>89.4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J23">
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -5797,7 +6222,7 @@
         <v>49002</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -5826,11 +6251,11 @@
         <v>1.9599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="11"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="6">
         <v>22.6</v>
       </c>
@@ -5853,11 +6278,11 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:11" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="10"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="3">
         <f>IF(NOT(ISBLANK(C27)), C24*EXP(C25*C27), "")</f>
         <v>21.792110271198268</v>
@@ -5889,11 +6314,11 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="10"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="8">
         <v>25</v>
       </c>
@@ -5916,11 +6341,11 @@
         <v>78400</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+    <row r="30" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="9">
         <f>(100*C29/C28)-100</f>
         <v>14.720418026892361</v>
@@ -5950,17 +6375,17 @@
         <v>2.3351283597764052</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -5977,11 +6402,11 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+    <row r="35" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A35" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="11"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -5998,11 +6423,11 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+    <row r="36" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A36" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="10"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -6042,19 +6467,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1B8C85-3DA4-434F-83AF-5F1A19563F16}">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -6075,12 +6505,15 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="V2">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -6106,7 +6539,11 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>B4+273.15</f>
+        <v>278.14999999999998</v>
+      </c>
       <c r="B4" s="2">
         <v>5</v>
       </c>
@@ -6136,7 +6573,11 @@
         <v>53.8</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" ref="A5:A22" si="0">B5+273.15</f>
+        <v>283.14999999999998</v>
+      </c>
       <c r="B5" s="2">
         <v>10</v>
       </c>
@@ -6159,14 +6600,18 @@
         <v>10720</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I22" si="0">J5*$J$23</f>
+        <f t="shared" ref="I5:I22" si="1">J5*$J$23</f>
         <v>58900</v>
       </c>
       <c r="J5">
         <v>58.9</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>288.14999999999998</v>
+      </c>
       <c r="B6" s="2">
         <v>15</v>
       </c>
@@ -6189,14 +6634,18 @@
         <v>12050</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65700</v>
       </c>
       <c r="J6">
         <v>65.7</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>289.14999999999998</v>
+      </c>
       <c r="B7" s="2">
         <v>16</v>
       </c>
@@ -6219,14 +6668,18 @@
         <v>12280</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>67200</v>
       </c>
       <c r="J7">
         <v>67.2</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>290.14999999999998</v>
+      </c>
       <c r="B8" s="2">
         <v>17</v>
       </c>
@@ -6249,14 +6702,18 @@
         <v>12590</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68700</v>
       </c>
       <c r="J8">
         <v>68.7</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>291.14999999999998</v>
+      </c>
       <c r="B9" s="2">
         <v>18</v>
       </c>
@@ -6279,14 +6736,18 @@
         <v>12900</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70100</v>
       </c>
       <c r="J9">
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>292.14999999999998</v>
+      </c>
       <c r="B10" s="2">
         <v>19</v>
       </c>
@@ -6309,14 +6770,18 @@
         <v>13190</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>71500</v>
       </c>
       <c r="J10">
         <v>71.5</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>293.14999999999998</v>
+      </c>
       <c r="B11" s="2">
         <v>20</v>
       </c>
@@ -6339,14 +6804,18 @@
         <v>13510</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>72900</v>
       </c>
       <c r="J11">
         <v>72.900000000000006</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>294.14999999999998</v>
+      </c>
       <c r="B12" s="2">
         <v>21</v>
       </c>
@@ -6369,14 +6838,18 @@
         <v>13810</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>74300</v>
       </c>
       <c r="J12">
         <v>74.3</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>295.14999999999998</v>
+      </c>
       <c r="B13" s="2">
         <v>22</v>
       </c>
@@ -6399,14 +6872,18 @@
         <v>14090</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>75800</v>
       </c>
       <c r="J13">
         <v>75.8</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>296.14999999999998</v>
+      </c>
       <c r="B14" s="2">
         <v>23</v>
       </c>
@@ -6429,14 +6906,18 @@
         <v>14350</v>
       </c>
       <c r="I14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>77200</v>
       </c>
       <c r="J14">
         <v>77.2</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>297.14999999999998</v>
+      </c>
       <c r="B15" s="2">
         <v>24</v>
       </c>
@@ -6459,14 +6940,18 @@
         <v>14690</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>78600</v>
       </c>
       <c r="J15">
         <v>78.599999999999994</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>298.14999999999998</v>
+      </c>
       <c r="B16" s="2">
         <v>25</v>
       </c>
@@ -6489,14 +6974,18 @@
         <v>15000</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80000</v>
       </c>
       <c r="J16">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>299.14999999999998</v>
+      </c>
       <c r="B17" s="2">
         <v>26</v>
       </c>
@@ -6519,14 +7008,18 @@
         <v>15280</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>81600</v>
       </c>
       <c r="J17">
         <v>81.599999999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>300.14999999999998</v>
+      </c>
       <c r="B18" s="2">
         <v>27</v>
       </c>
@@ -6549,14 +7042,18 @@
         <v>15510</v>
       </c>
       <c r="I18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>83100</v>
       </c>
       <c r="J18">
         <v>83.1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>301.14999999999998</v>
+      </c>
       <c r="B19" s="2">
         <v>28</v>
       </c>
@@ -6579,14 +7076,18 @@
         <v>15820</v>
       </c>
       <c r="I19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84700</v>
       </c>
       <c r="J19">
         <v>84.7</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>302.14999999999998</v>
+      </c>
       <c r="B20" s="2">
         <v>29</v>
       </c>
@@ -6609,14 +7110,18 @@
         <v>16130</v>
       </c>
       <c r="I20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86200</v>
       </c>
       <c r="J20">
         <v>86.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>303.14999999999998</v>
+      </c>
       <c r="B21" s="2">
         <v>30</v>
       </c>
@@ -6639,14 +7144,18 @@
         <v>16450</v>
       </c>
       <c r="I21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>87700</v>
       </c>
       <c r="J21">
         <v>87.7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>304.14999999999998</v>
+      </c>
       <c r="B22" s="2">
         <v>31</v>
       </c>
@@ -6669,19 +7178,19 @@
         <v>16770</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>89400</v>
       </c>
       <c r="J22">
         <v>89.4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J23">
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -6689,28 +7198,28 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>13.465999999999999</v>
+        <v>4.0399999999999998E-2</v>
       </c>
       <c r="D24">
-        <v>55.853999999999999</v>
+        <v>0.68820000000000003</v>
       </c>
       <c r="E24">
-        <v>254.83</v>
+        <v>0.54630000000000001</v>
       </c>
       <c r="F24">
-        <v>1110.0999999999999</v>
+        <v>1.3501000000000001</v>
       </c>
       <c r="G24">
-        <v>1624.1</v>
+        <v>5.0342000000000002</v>
       </c>
       <c r="H24">
-        <v>8564.4</v>
+        <v>22.571999999999999</v>
       </c>
       <c r="I24">
-        <v>49002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>231.34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -6739,11 +7248,11 @@
         <v>1.9599999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+    <row r="27" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="11"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="6">
         <v>22.8</v>
       </c>
@@ -6767,11 +7276,11 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="10"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="8">
         <v>35.799999999999997</v>
       </c>
@@ -6794,77 +7303,77 @@
         <v>75200</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:11" s="5" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="10"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="3">
-        <f>IF(NOT(ISBLANK(C27)), C24*EXP(C25*C27), "")</f>
-        <v>21.885142679289942</v>
+        <f>IF(NOT(ISBLANK(C27)), C24*EXP(C25*(C27+273.15)), "")</f>
+        <v>22.083031451520686</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" ref="D29:I29" si="1">IF(NOT(ISBLANK(D27)), D24*EXP(D25*D27), "")</f>
-        <v>79.979563305892157</v>
+        <f t="shared" ref="D29:I29" si="2">IF(NOT(ISBLANK(D27)), D24*EXP(D25*(D27+273.15)), "")</f>
+        <v>80.083449870600745</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" si="1"/>
-        <v>415.23584340432336</v>
+        <f t="shared" si="2"/>
+        <v>415.52301190975328</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" si="1"/>
-        <v>1883.9113131685938</v>
+        <f t="shared" si="2"/>
+        <v>1898.0240755447328</v>
       </c>
       <c r="G29" s="3">
-        <f t="shared" si="1"/>
-        <v>2650.6113624414397</v>
+        <f t="shared" si="2"/>
+        <v>2616.4039760779833</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="1"/>
-        <v>13774.982392033568</v>
+        <f t="shared" si="2"/>
+        <v>13997.306540263537</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" si="1"/>
-        <v>75271.465111520898</v>
+        <f t="shared" si="2"/>
+        <v>75121.981390131928</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+    <row r="30" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="9">
-        <f t="shared" ref="C30:I30" si="2">(100*C28/C29)-100</f>
-        <v>63.581295880139635</v>
+        <f t="shared" ref="C30:I30" si="3">(100*C28/C29)-100</f>
+        <v>62.11542368443591</v>
       </c>
       <c r="D30" s="9">
-        <f t="shared" si="2"/>
-        <v>9.7780437537494151</v>
+        <f t="shared" si="3"/>
+        <v>9.6356365040063849</v>
       </c>
       <c r="E30" s="9">
-        <f t="shared" si="2"/>
-        <v>2.5922994767085612</v>
+        <f t="shared" si="3"/>
+        <v>2.5213978022767662</v>
       </c>
       <c r="F30" s="9">
-        <f t="shared" si="2"/>
-        <v>3.9857867144028631</v>
+        <f t="shared" si="3"/>
+        <v>3.2126001582865626</v>
       </c>
       <c r="G30" s="9">
-        <f t="shared" si="2"/>
-        <v>-0.77760786562292594</v>
+        <f t="shared" si="3"/>
+        <v>0.51964543879027758</v>
       </c>
       <c r="H30" s="9">
-        <f t="shared" si="2"/>
-        <v>1.0527607501719984</v>
+        <f t="shared" si="3"/>
+        <v>-0.55229582949522182</v>
       </c>
       <c r="I30" s="9">
-        <f t="shared" si="2"/>
-        <v>-9.4943165268560392E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.10385589999670231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -6872,12 +7381,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -6894,11 +7403,11 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+    <row r="35" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A35" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="11"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -6915,29 +7424,29 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+    <row r="36" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+      <c r="A36" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="10"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3">
         <f>IF(NOT(ISBLANK(F35)), F24*EXP(F25*F35), "")</f>
-        <v>1969.2053807568627</v>
+        <v>2.3949411625617878</v>
       </c>
       <c r="G36" s="3">
         <f>IF(NOT(ISBLANK(G35)), G24*EXP(G25*G35), "")</f>
-        <v>2638.6140973673614</v>
+        <v>8.1788751240482558</v>
       </c>
       <c r="H36" s="3">
         <f>IF(NOT(ISBLANK(H35)), H24*EXP(H25*H35), "")</f>
-        <v>14047.916272625975</v>
+        <v>37.024142509190781</v>
       </c>
       <c r="I36" s="3">
         <f>IF(NOT(ISBLANK(I35)), I24*EXP(I25*I35), "")</f>
-        <v>76461.023449634566</v>
+        <v>360.97492275495819</v>
       </c>
     </row>
   </sheetData>
@@ -6953,4 +7462,933 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F487083-BFED-5542-BCDF-A426D7FF26E9}">
+  <dimension ref="B1:E57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+    </row>
+    <row r="2" spans="2:5" s="26" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="18">
+        <v>0</v>
+      </c>
+      <c r="C3" s="27">
+        <v>0</v>
+      </c>
+      <c r="D3" s="20">
+        <v>0</v>
+      </c>
+      <c r="E3" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="10">
+        <v>200</v>
+      </c>
+      <c r="C4" s="12">
+        <f t="shared" ref="C4:C18" si="0">D4*0.006895</f>
+        <v>13.790000000000001</v>
+      </c>
+      <c r="D4" s="11">
+        <f>B4*10</f>
+        <v>2000</v>
+      </c>
+      <c r="E4" s="13">
+        <f>D4/14.7</f>
+        <v>136.0544217687075</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="10">
+        <v>400</v>
+      </c>
+      <c r="C5" s="12">
+        <f t="shared" si="0"/>
+        <v>27.580000000000002</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" ref="D5:D56" si="1">B5*10</f>
+        <v>4000</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" ref="E5:E56" si="2">D5/14.7</f>
+        <v>272.108843537415</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="10">
+        <v>600</v>
+      </c>
+      <c r="C6" s="12">
+        <f t="shared" si="0"/>
+        <v>41.37</v>
+      </c>
+      <c r="D6" s="11">
+        <f t="shared" si="1"/>
+        <v>6000</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="2"/>
+        <v>408.16326530612247</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="10">
+        <v>800</v>
+      </c>
+      <c r="C7" s="12">
+        <f t="shared" si="0"/>
+        <v>55.160000000000004</v>
+      </c>
+      <c r="D7" s="11">
+        <f t="shared" si="1"/>
+        <v>8000</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="2"/>
+        <v>544.21768707483</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="22">
+        <v>1000</v>
+      </c>
+      <c r="C8" s="23">
+        <f t="shared" si="0"/>
+        <v>68.95</v>
+      </c>
+      <c r="D8" s="24">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="E8" s="25">
+        <f t="shared" si="2"/>
+        <v>680.27210884353747</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="13" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="18">
+        <v>1200</v>
+      </c>
+      <c r="C9" s="19">
+        <f t="shared" si="0"/>
+        <v>82.74</v>
+      </c>
+      <c r="D9" s="20">
+        <f t="shared" si="1"/>
+        <v>12000</v>
+      </c>
+      <c r="E9" s="21">
+        <f t="shared" si="2"/>
+        <v>816.32653061224494</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="10">
+        <v>1400</v>
+      </c>
+      <c r="C10" s="12">
+        <f t="shared" si="0"/>
+        <v>96.53</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="1"/>
+        <v>14000</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="2"/>
+        <v>952.38095238095241</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="10">
+        <v>1600</v>
+      </c>
+      <c r="C11" s="12">
+        <f t="shared" si="0"/>
+        <v>110.32000000000001</v>
+      </c>
+      <c r="D11" s="11">
+        <f t="shared" si="1"/>
+        <v>16000</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="2"/>
+        <v>1088.43537414966</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="10">
+        <v>1800</v>
+      </c>
+      <c r="C12" s="12">
+        <f t="shared" si="0"/>
+        <v>124.11</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" si="1"/>
+        <v>18000</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="2"/>
+        <v>1224.4897959183675</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="22">
+        <v>2000</v>
+      </c>
+      <c r="C13" s="23">
+        <f t="shared" si="0"/>
+        <v>137.9</v>
+      </c>
+      <c r="D13" s="24">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+      <c r="E13" s="25">
+        <f t="shared" si="2"/>
+        <v>1360.5442176870749</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="13" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="18">
+        <v>2200</v>
+      </c>
+      <c r="C14" s="19">
+        <f t="shared" si="0"/>
+        <v>151.69</v>
+      </c>
+      <c r="D14" s="20">
+        <f t="shared" si="1"/>
+        <v>22000</v>
+      </c>
+      <c r="E14" s="21">
+        <f t="shared" si="2"/>
+        <v>1496.5986394557824</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="10">
+        <v>2400</v>
+      </c>
+      <c r="C15" s="12">
+        <f t="shared" si="0"/>
+        <v>165.48</v>
+      </c>
+      <c r="D15" s="11">
+        <f t="shared" si="1"/>
+        <v>24000</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" si="2"/>
+        <v>1632.6530612244899</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="10">
+        <v>2600</v>
+      </c>
+      <c r="C16" s="12">
+        <f t="shared" si="0"/>
+        <v>179.27</v>
+      </c>
+      <c r="D16" s="11">
+        <f t="shared" si="1"/>
+        <v>26000</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="2"/>
+        <v>1768.7074829931973</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="10">
+        <v>2800</v>
+      </c>
+      <c r="C17" s="12">
+        <f t="shared" si="0"/>
+        <v>193.06</v>
+      </c>
+      <c r="D17" s="11">
+        <f t="shared" si="1"/>
+        <v>28000</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="2"/>
+        <v>1904.7619047619048</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="14">
+        <v>3000</v>
+      </c>
+      <c r="C18" s="15">
+        <f t="shared" si="0"/>
+        <v>206.85</v>
+      </c>
+      <c r="D18" s="16">
+        <f t="shared" si="1"/>
+        <v>30000</v>
+      </c>
+      <c r="E18" s="17">
+        <f t="shared" si="2"/>
+        <v>2040.8163265306123</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
+    </row>
+    <row r="20" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="18">
+        <v>3200</v>
+      </c>
+      <c r="C20" s="19">
+        <f t="shared" ref="C20:C34" si="3">D20*0.006895</f>
+        <v>220.64000000000001</v>
+      </c>
+      <c r="D20" s="20">
+        <f t="shared" si="1"/>
+        <v>32000</v>
+      </c>
+      <c r="E20" s="21">
+        <f t="shared" si="2"/>
+        <v>2176.87074829932</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="10">
+        <v>3400</v>
+      </c>
+      <c r="C21" s="12">
+        <f t="shared" si="3"/>
+        <v>234.43</v>
+      </c>
+      <c r="D21" s="11">
+        <f t="shared" si="1"/>
+        <v>34000</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" si="2"/>
+        <v>2312.9251700680275</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="10">
+        <v>3600</v>
+      </c>
+      <c r="C22" s="12">
+        <f t="shared" si="3"/>
+        <v>248.22</v>
+      </c>
+      <c r="D22" s="11">
+        <f t="shared" si="1"/>
+        <v>36000</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="2"/>
+        <v>2448.9795918367349</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="10">
+        <v>3800</v>
+      </c>
+      <c r="C23" s="12">
+        <f t="shared" si="3"/>
+        <v>262.01</v>
+      </c>
+      <c r="D23" s="11">
+        <f t="shared" si="1"/>
+        <v>38000</v>
+      </c>
+      <c r="E23" s="13">
+        <f t="shared" si="2"/>
+        <v>2585.0340136054424</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="22">
+        <v>4000</v>
+      </c>
+      <c r="C24" s="23">
+        <f t="shared" si="3"/>
+        <v>275.8</v>
+      </c>
+      <c r="D24" s="24">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="E24" s="25">
+        <f t="shared" si="2"/>
+        <v>2721.0884353741499</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="13" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="18">
+        <v>4200</v>
+      </c>
+      <c r="C25" s="19">
+        <f t="shared" si="3"/>
+        <v>289.59000000000003</v>
+      </c>
+      <c r="D25" s="20">
+        <f t="shared" si="1"/>
+        <v>42000</v>
+      </c>
+      <c r="E25" s="21">
+        <f t="shared" si="2"/>
+        <v>2857.1428571428573</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="10">
+        <v>4400</v>
+      </c>
+      <c r="C26" s="12">
+        <f t="shared" si="3"/>
+        <v>303.38</v>
+      </c>
+      <c r="D26" s="11">
+        <f t="shared" si="1"/>
+        <v>44000</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="2"/>
+        <v>2993.1972789115648</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="10">
+        <v>4600</v>
+      </c>
+      <c r="C27" s="12">
+        <f t="shared" si="3"/>
+        <v>317.17</v>
+      </c>
+      <c r="D27" s="11">
+        <f t="shared" si="1"/>
+        <v>46000</v>
+      </c>
+      <c r="E27" s="13">
+        <f t="shared" si="2"/>
+        <v>3129.2517006802723</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="10">
+        <v>4800</v>
+      </c>
+      <c r="C28" s="12">
+        <f t="shared" si="3"/>
+        <v>330.96</v>
+      </c>
+      <c r="D28" s="11">
+        <f t="shared" si="1"/>
+        <v>48000</v>
+      </c>
+      <c r="E28" s="13">
+        <f t="shared" si="2"/>
+        <v>3265.3061224489797</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="22">
+        <v>5000</v>
+      </c>
+      <c r="C29" s="23">
+        <f t="shared" si="3"/>
+        <v>344.75</v>
+      </c>
+      <c r="D29" s="24">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="E29" s="25">
+        <f t="shared" si="2"/>
+        <v>3401.3605442176872</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="13" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="18">
+        <v>5200</v>
+      </c>
+      <c r="C30" s="19">
+        <f t="shared" si="3"/>
+        <v>358.54</v>
+      </c>
+      <c r="D30" s="20">
+        <f t="shared" si="1"/>
+        <v>52000</v>
+      </c>
+      <c r="E30" s="21">
+        <f t="shared" si="2"/>
+        <v>3537.4149659863947</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="10">
+        <v>5400</v>
+      </c>
+      <c r="C31" s="12">
+        <f t="shared" si="3"/>
+        <v>372.33</v>
+      </c>
+      <c r="D31" s="11">
+        <f t="shared" si="1"/>
+        <v>54000</v>
+      </c>
+      <c r="E31" s="13">
+        <f t="shared" si="2"/>
+        <v>3673.4693877551022</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="10">
+        <v>5600</v>
+      </c>
+      <c r="C32" s="12">
+        <f t="shared" si="3"/>
+        <v>386.12</v>
+      </c>
+      <c r="D32" s="11">
+        <f t="shared" si="1"/>
+        <v>56000</v>
+      </c>
+      <c r="E32" s="13">
+        <f t="shared" si="2"/>
+        <v>3809.5238095238096</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="10">
+        <v>5800</v>
+      </c>
+      <c r="C33" s="12">
+        <f t="shared" si="3"/>
+        <v>399.91</v>
+      </c>
+      <c r="D33" s="11">
+        <f t="shared" si="1"/>
+        <v>58000</v>
+      </c>
+      <c r="E33" s="13">
+        <f t="shared" si="2"/>
+        <v>3945.5782312925171</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="14">
+        <v>6000</v>
+      </c>
+      <c r="C34" s="15">
+        <f t="shared" si="3"/>
+        <v>413.7</v>
+      </c>
+      <c r="D34" s="16">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="E34" s="17">
+        <f t="shared" si="2"/>
+        <v>4081.6326530612246</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="33"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="36"/>
+    </row>
+    <row r="36" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="18">
+        <v>6200</v>
+      </c>
+      <c r="C36" s="19">
+        <f t="shared" ref="C36:C50" si="4">D36*0.006895</f>
+        <v>427.49</v>
+      </c>
+      <c r="D36" s="20">
+        <f t="shared" si="1"/>
+        <v>62000</v>
+      </c>
+      <c r="E36" s="21">
+        <f t="shared" si="2"/>
+        <v>4217.6870748299325</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="10">
+        <v>6400</v>
+      </c>
+      <c r="C37" s="12">
+        <f t="shared" si="4"/>
+        <v>441.28000000000003</v>
+      </c>
+      <c r="D37" s="11">
+        <f t="shared" si="1"/>
+        <v>64000</v>
+      </c>
+      <c r="E37" s="13">
+        <f t="shared" si="2"/>
+        <v>4353.74149659864</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="10">
+        <v>6600</v>
+      </c>
+      <c r="C38" s="12">
+        <f t="shared" si="4"/>
+        <v>455.07</v>
+      </c>
+      <c r="D38" s="11">
+        <f t="shared" si="1"/>
+        <v>66000</v>
+      </c>
+      <c r="E38" s="13">
+        <f t="shared" si="2"/>
+        <v>4489.7959183673474</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="10">
+        <v>6800</v>
+      </c>
+      <c r="C39" s="12">
+        <f t="shared" si="4"/>
+        <v>468.86</v>
+      </c>
+      <c r="D39" s="11">
+        <f t="shared" si="1"/>
+        <v>68000</v>
+      </c>
+      <c r="E39" s="13">
+        <f t="shared" si="2"/>
+        <v>4625.8503401360549</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="22">
+        <v>7000</v>
+      </c>
+      <c r="C40" s="23">
+        <f t="shared" si="4"/>
+        <v>482.65000000000003</v>
+      </c>
+      <c r="D40" s="24">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="E40" s="25">
+        <f t="shared" si="2"/>
+        <v>4761.9047619047624</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="13" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="18">
+        <v>7200</v>
+      </c>
+      <c r="C41" s="19">
+        <f t="shared" si="4"/>
+        <v>496.44</v>
+      </c>
+      <c r="D41" s="20">
+        <f t="shared" si="1"/>
+        <v>72000</v>
+      </c>
+      <c r="E41" s="21">
+        <f t="shared" si="2"/>
+        <v>4897.9591836734699</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="10">
+        <v>7400</v>
+      </c>
+      <c r="C42" s="12">
+        <f t="shared" si="4"/>
+        <v>510.23</v>
+      </c>
+      <c r="D42" s="11">
+        <f t="shared" si="1"/>
+        <v>74000</v>
+      </c>
+      <c r="E42" s="13">
+        <f t="shared" si="2"/>
+        <v>5034.0136054421773</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="10">
+        <v>7600</v>
+      </c>
+      <c r="C43" s="12">
+        <f t="shared" si="4"/>
+        <v>524.02</v>
+      </c>
+      <c r="D43" s="11">
+        <f t="shared" si="1"/>
+        <v>76000</v>
+      </c>
+      <c r="E43" s="13">
+        <f t="shared" si="2"/>
+        <v>5170.0680272108848</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="10">
+        <v>7800</v>
+      </c>
+      <c r="C44" s="12">
+        <f t="shared" si="4"/>
+        <v>537.81000000000006</v>
+      </c>
+      <c r="D44" s="11">
+        <f t="shared" si="1"/>
+        <v>78000</v>
+      </c>
+      <c r="E44" s="13">
+        <f t="shared" si="2"/>
+        <v>5306.1224489795923</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="22">
+        <v>8000</v>
+      </c>
+      <c r="C45" s="23">
+        <f t="shared" si="4"/>
+        <v>551.6</v>
+      </c>
+      <c r="D45" s="24">
+        <f t="shared" si="1"/>
+        <v>80000</v>
+      </c>
+      <c r="E45" s="25">
+        <f t="shared" si="2"/>
+        <v>5442.1768707482997</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="13" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="18">
+        <v>8200</v>
+      </c>
+      <c r="C46" s="19">
+        <f t="shared" si="4"/>
+        <v>565.39</v>
+      </c>
+      <c r="D46" s="20">
+        <f t="shared" si="1"/>
+        <v>82000</v>
+      </c>
+      <c r="E46" s="21">
+        <f t="shared" si="2"/>
+        <v>5578.2312925170072</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="10">
+        <v>8400</v>
+      </c>
+      <c r="C47" s="12">
+        <f t="shared" si="4"/>
+        <v>579.18000000000006</v>
+      </c>
+      <c r="D47" s="11">
+        <f t="shared" si="1"/>
+        <v>84000</v>
+      </c>
+      <c r="E47" s="13">
+        <f t="shared" si="2"/>
+        <v>5714.2857142857147</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="10">
+        <v>8600</v>
+      </c>
+      <c r="C48" s="12">
+        <f t="shared" si="4"/>
+        <v>592.97</v>
+      </c>
+      <c r="D48" s="11">
+        <f t="shared" si="1"/>
+        <v>86000</v>
+      </c>
+      <c r="E48" s="13">
+        <f t="shared" si="2"/>
+        <v>5850.3401360544221</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="10">
+        <v>8800</v>
+      </c>
+      <c r="C49" s="12">
+        <f t="shared" si="4"/>
+        <v>606.76</v>
+      </c>
+      <c r="D49" s="11">
+        <f t="shared" si="1"/>
+        <v>88000</v>
+      </c>
+      <c r="E49" s="13">
+        <f t="shared" si="2"/>
+        <v>5986.3945578231296</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="14">
+        <v>9000</v>
+      </c>
+      <c r="C50" s="15">
+        <f t="shared" si="4"/>
+        <v>620.54999999999995</v>
+      </c>
+      <c r="D50" s="16">
+        <f t="shared" si="1"/>
+        <v>90000</v>
+      </c>
+      <c r="E50" s="17">
+        <f t="shared" si="2"/>
+        <v>6122.4489795918371</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="33"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="36"/>
+    </row>
+    <row r="52" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="18">
+        <v>9200</v>
+      </c>
+      <c r="C52" s="19">
+        <f>D52*0.006895</f>
+        <v>634.34</v>
+      </c>
+      <c r="D52" s="20">
+        <f t="shared" si="1"/>
+        <v>92000</v>
+      </c>
+      <c r="E52" s="21">
+        <f t="shared" si="2"/>
+        <v>6258.5034013605446</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="10">
+        <v>9400</v>
+      </c>
+      <c r="C53" s="12">
+        <f>D53*0.006895</f>
+        <v>648.13</v>
+      </c>
+      <c r="D53" s="11">
+        <f t="shared" si="1"/>
+        <v>94000</v>
+      </c>
+      <c r="E53" s="13">
+        <f t="shared" si="2"/>
+        <v>6394.557823129252</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="10">
+        <v>9600</v>
+      </c>
+      <c r="C54" s="12">
+        <f>D54*0.006895</f>
+        <v>661.92</v>
+      </c>
+      <c r="D54" s="11">
+        <f t="shared" si="1"/>
+        <v>96000</v>
+      </c>
+      <c r="E54" s="13">
+        <f t="shared" si="2"/>
+        <v>6530.6122448979595</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="10">
+        <v>9800</v>
+      </c>
+      <c r="C55" s="12">
+        <f>D55*0.006895</f>
+        <v>675.71</v>
+      </c>
+      <c r="D55" s="11">
+        <f t="shared" si="1"/>
+        <v>98000</v>
+      </c>
+      <c r="E55" s="13">
+        <f t="shared" si="2"/>
+        <v>6666.666666666667</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="22">
+        <v>10000</v>
+      </c>
+      <c r="C56" s="23">
+        <f>D56*0.006895</f>
+        <v>689.5</v>
+      </c>
+      <c r="D56" s="24">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="E56" s="25">
+        <f t="shared" si="2"/>
+        <v>6802.7210884353744</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>